<commit_message>
Try join participants with surveys and discover typo and missing elems in the data
</commit_message>
<xml_diff>
--- a/data/Participants.xlsx
+++ b/data/Participants.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28209"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="472" documentId="11_9D5355BF84DCCE53631DEA188F31F45B3A7E0439" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68066ECE-9839-480D-96C8-35C96F774FD8}"/>
+  <xr:revisionPtr revIDLastSave="616" documentId="11_9D5355BF84DCCE53631DEA188F31F45B3A7E0439" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0B9E3F4-3E5E-4F49-837F-DC805A14BBCF}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="275">
   <si>
     <t>Grupa dz.</t>
   </si>
@@ -51,6 +51,9 @@
     <t>Inspiracje AI</t>
   </si>
   <si>
+    <t>Matryce</t>
+  </si>
+  <si>
     <t>EAG</t>
   </si>
   <si>
@@ -69,6 +72,9 @@
     <t>1A_11_13</t>
   </si>
   <si>
+    <t>M_1A</t>
+  </si>
+  <si>
     <t>1B</t>
   </si>
   <si>
@@ -81,6 +87,9 @@
     <t>1B_11_18</t>
   </si>
   <si>
+    <t>M_1B</t>
+  </si>
+  <si>
     <t>2A</t>
   </si>
   <si>
@@ -93,6 +102,9 @@
     <t>2A_11_16</t>
   </si>
   <si>
+    <t>M_2A</t>
+  </si>
+  <si>
     <t>2B</t>
   </si>
   <si>
@@ -105,6 +117,9 @@
     <t>2B_11_18</t>
   </si>
   <si>
+    <t>M_2B</t>
+  </si>
+  <si>
     <t>3A</t>
   </si>
   <si>
@@ -117,6 +132,9 @@
     <t>3A_11_20</t>
   </si>
   <si>
+    <t>M_3A</t>
+  </si>
+  <si>
     <t>3B</t>
   </si>
   <si>
@@ -129,6 +147,12 @@
     <t>3B_11_20</t>
   </si>
   <si>
+    <t>M_3B</t>
+  </si>
+  <si>
+    <t>ma więcej</t>
+  </si>
+  <si>
     <t>4A</t>
   </si>
   <si>
@@ -141,6 +165,9 @@
     <t>4A_11_20</t>
   </si>
   <si>
+    <t>M_4A</t>
+  </si>
+  <si>
     <t>4B</t>
   </si>
   <si>
@@ -153,16 +180,25 @@
     <t>4B_11_20</t>
   </si>
   <si>
+    <t>M_4B</t>
+  </si>
+  <si>
     <t>5A</t>
   </si>
   <si>
     <t>Nela Salwin</t>
   </si>
   <si>
-    <t>5A_1–10</t>
-  </si>
-  <si>
-    <t>5A_11_20</t>
+    <t>5A_1–9</t>
+  </si>
+  <si>
+    <t>5A_11_18</t>
+  </si>
+  <si>
+    <t>M_5A</t>
+  </si>
+  <si>
+    <t>brakuje 5A_5</t>
   </si>
   <si>
     <t>5B</t>
@@ -171,10 +207,16 @@
     <t>Oliwia Konieczna</t>
   </si>
   <si>
-    <t>5B_1–10</t>
-  </si>
-  <si>
-    <t>5B_11_20</t>
+    <t>5B_1–8</t>
+  </si>
+  <si>
+    <t>5B_11_17</t>
+  </si>
+  <si>
+    <t>M_5B</t>
+  </si>
+  <si>
+    <t>brakuje 5B_8</t>
   </si>
   <si>
     <t>6A</t>
@@ -189,6 +231,9 @@
     <t>6A_11_20</t>
   </si>
   <si>
+    <t>brak danych</t>
+  </si>
+  <si>
     <t>6B</t>
   </si>
   <si>
@@ -198,7 +243,10 @@
     <t>6B_1–10</t>
   </si>
   <si>
-    <t>6B_11_20</t>
+    <t>6B_11_19</t>
+  </si>
+  <si>
+    <t>M_6B</t>
   </si>
   <si>
     <t>7A</t>
@@ -213,16 +261,22 @@
     <t>7A_11_20</t>
   </si>
   <si>
+    <t>M_7A</t>
+  </si>
+  <si>
     <t>7B</t>
   </si>
   <si>
     <t>Julia Osuch</t>
   </si>
   <si>
-    <t>7B_1–10</t>
-  </si>
-  <si>
-    <t>7B_11_20</t>
+    <t>7B_1–9</t>
+  </si>
+  <si>
+    <t>7B_11_12</t>
+  </si>
+  <si>
+    <t>M_7B</t>
   </si>
   <si>
     <t>7C</t>
@@ -237,6 +291,9 @@
     <t>7C_11_20</t>
   </si>
   <si>
+    <t>M_7C</t>
+  </si>
+  <si>
     <t>MM</t>
   </si>
   <si>
@@ -258,7 +315,7 @@
     <t>8A_11_20</t>
   </si>
   <si>
-    <t>ma więcej</t>
+    <t>M_8A</t>
   </si>
   <si>
     <t>8B</t>
@@ -276,6 +333,9 @@
     <t>8B_11_20</t>
   </si>
   <si>
+    <t>M_8B</t>
+  </si>
+  <si>
     <t>9A</t>
   </si>
   <si>
@@ -288,6 +348,9 @@
     <t>9A_11_19</t>
   </si>
   <si>
+    <t>M_9A</t>
+  </si>
+  <si>
     <t>9B</t>
   </si>
   <si>
@@ -300,6 +363,9 @@
     <t>9B_11_17</t>
   </si>
   <si>
+    <t>M_9B</t>
+  </si>
+  <si>
     <t>10A</t>
   </si>
   <si>
@@ -312,6 +378,9 @@
     <t>10A_11_16</t>
   </si>
   <si>
+    <t>M_10A</t>
+  </si>
+  <si>
     <t>10B</t>
   </si>
   <si>
@@ -324,6 +393,9 @@
     <t>10B_11_17</t>
   </si>
   <si>
+    <t>M_10B</t>
+  </si>
+  <si>
     <t>11A</t>
   </si>
   <si>
@@ -336,6 +408,9 @@
     <t>11A_11_20</t>
   </si>
   <si>
+    <t>M_11A</t>
+  </si>
+  <si>
     <t>11B</t>
   </si>
   <si>
@@ -348,6 +423,9 @@
     <t>11B_11_18</t>
   </si>
   <si>
+    <t>M_11B</t>
+  </si>
+  <si>
     <t>12A</t>
   </si>
   <si>
@@ -360,6 +438,9 @@
     <t>12A_11_20</t>
   </si>
   <si>
+    <t>M_12A</t>
+  </si>
+  <si>
     <t>12B</t>
   </si>
   <si>
@@ -372,6 +453,9 @@
     <t>12B_11_17</t>
   </si>
   <si>
+    <t>M_12B</t>
+  </si>
+  <si>
     <t>nie mogę otworzyć niektórych plików</t>
   </si>
   <si>
@@ -387,6 +471,9 @@
     <t>13A_11_20</t>
   </si>
   <si>
+    <t>M_13A</t>
+  </si>
+  <si>
     <t>13B</t>
   </si>
   <si>
@@ -399,6 +486,9 @@
     <t>13B_11_20</t>
   </si>
   <si>
+    <t>M_13B</t>
+  </si>
+  <si>
     <t>14A</t>
   </si>
   <si>
@@ -411,6 +501,9 @@
     <t>14A_11_20</t>
   </si>
   <si>
+    <t>M_14A</t>
+  </si>
+  <si>
     <t>14B</t>
   </si>
   <si>
@@ -423,6 +516,9 @@
     <t>14B_11_20</t>
   </si>
   <si>
+    <t>M_14B</t>
+  </si>
+  <si>
     <t>15A</t>
   </si>
   <si>
@@ -435,6 +531,9 @@
     <t>15A_11_16</t>
   </si>
   <si>
+    <t>M_15A</t>
+  </si>
+  <si>
     <t>15B</t>
   </si>
   <si>
@@ -447,6 +546,9 @@
     <t>15B_11_16</t>
   </si>
   <si>
+    <t>M_15B</t>
+  </si>
+  <si>
     <t>16A</t>
   </si>
   <si>
@@ -459,6 +561,9 @@
     <t>16A_11_20</t>
   </si>
   <si>
+    <t>M_16A</t>
+  </si>
+  <si>
     <t>16B</t>
   </si>
   <si>
@@ -471,6 +576,9 @@
     <t>16B_11_13</t>
   </si>
   <si>
+    <t>M_16B</t>
+  </si>
+  <si>
     <t>2.2 (I st)</t>
   </si>
   <si>
@@ -486,6 +594,9 @@
     <t>17A_11-13</t>
   </si>
   <si>
+    <t>M_17A</t>
+  </si>
+  <si>
     <t>17B</t>
   </si>
   <si>
@@ -498,6 +609,9 @@
     <t>17B_11-20</t>
   </si>
   <si>
+    <t>M_17B</t>
+  </si>
+  <si>
     <t>18A</t>
   </si>
   <si>
@@ -510,6 +624,9 @@
     <t>18A_11-20</t>
   </si>
   <si>
+    <t>M_18A</t>
+  </si>
+  <si>
     <t>18B</t>
   </si>
   <si>
@@ -522,6 +639,9 @@
     <t>18B_11-20</t>
   </si>
   <si>
+    <t>M_18B</t>
+  </si>
+  <si>
     <t>19A</t>
   </si>
   <si>
@@ -534,6 +654,9 @@
     <t>19A_11-20</t>
   </si>
   <si>
+    <t>M_19A</t>
+  </si>
+  <si>
     <t>19B</t>
   </si>
   <si>
@@ -546,6 +669,9 @@
     <t>19B_11-20</t>
   </si>
   <si>
+    <t>M_19B</t>
+  </si>
+  <si>
     <t>20A</t>
   </si>
   <si>
@@ -558,6 +684,9 @@
     <t>20A_11-19</t>
   </si>
   <si>
+    <t>M_20A</t>
+  </si>
+  <si>
     <t>20B</t>
   </si>
   <si>
@@ -570,6 +699,9 @@
     <t>20B_11-20</t>
   </si>
   <si>
+    <t>M_20B</t>
+  </si>
+  <si>
     <t>21A</t>
   </si>
   <si>
@@ -582,6 +714,9 @@
     <t>21A_11-20</t>
   </si>
   <si>
+    <t>M_21A</t>
+  </si>
+  <si>
     <t>21B</t>
   </si>
   <si>
@@ -594,6 +729,9 @@
     <t>21B_11-20</t>
   </si>
   <si>
+    <t>M_21B</t>
+  </si>
+  <si>
     <t>22A</t>
   </si>
   <si>
@@ -606,6 +744,9 @@
     <t>22A_11-20</t>
   </si>
   <si>
+    <t>M_22A</t>
+  </si>
+  <si>
     <t>22B</t>
   </si>
   <si>
@@ -618,6 +759,9 @@
     <t>22B_11-20</t>
   </si>
   <si>
+    <t>M_22B</t>
+  </si>
+  <si>
     <t>23A</t>
   </si>
   <si>
@@ -630,6 +774,9 @@
     <t>23A_11-20</t>
   </si>
   <si>
+    <t>M_23A</t>
+  </si>
+  <si>
     <t>23B</t>
   </si>
   <si>
@@ -642,6 +789,9 @@
     <t>23B_11-20</t>
   </si>
   <si>
+    <t>M_23B</t>
+  </si>
+  <si>
     <t>24A</t>
   </si>
   <si>
@@ -654,6 +804,9 @@
     <t>24A_11-20</t>
   </si>
   <si>
+    <t>M_24A</t>
+  </si>
+  <si>
     <t>24B</t>
   </si>
   <si>
@@ -666,6 +819,9 @@
     <t>24B_11-20</t>
   </si>
   <si>
+    <t>M_24B</t>
+  </si>
+  <si>
     <t>Sapozhnykov Daniil</t>
   </si>
   <si>
@@ -675,6 +831,9 @@
     <t>25_11-20</t>
   </si>
   <si>
+    <t>M_25A</t>
+  </si>
+  <si>
     <t>Mądrawska Oliwia</t>
   </si>
   <si>
@@ -684,6 +843,9 @@
     <t>26_11-14</t>
   </si>
   <si>
+    <t>M_26A</t>
+  </si>
+  <si>
     <t>Rybarczyk Klaudia</t>
   </si>
   <si>
@@ -691,13 +853,16 @@
   </si>
   <si>
     <t>27_11-20</t>
+  </si>
+  <si>
+    <t>M_27A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -708,6 +873,13 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -800,7 +972,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -827,6 +999,22 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1168,10 +1356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I54"/>
+  <dimension ref="A2:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1182,9 +1370,10 @@
     <col min="6" max="6" width="34.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1203,1372 +1392,1544 @@
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>12</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>17</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>22</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E6" s="3">
         <v>2</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>27</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E7" s="3">
         <v>3</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>32</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E8" s="3">
         <v>3</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>35</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E9" s="3">
         <v>4</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>41</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E10" s="3">
         <v>4</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>46</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E11" s="3">
         <v>5</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>51</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E12" s="3">
         <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>57</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="11">
         <v>6</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="3">
-        <v>6</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="F13" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="15"/>
+      <c r="J13" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="E14" s="3">
         <v>6</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>68</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="E15" s="3">
         <v>7</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>73</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="E16" s="3">
         <v>7</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>78</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="E17" s="3">
         <v>7</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>83</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="I18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>93</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="J18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="I19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>99</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="J19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>104</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>109</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>114</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>119</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>124</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>129</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="I26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>134</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="J26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I27" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>139</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="J27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>114</v>
+        <v>142</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>145</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>120</v>
+        <v>149</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>150</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>122</v>
+        <v>152</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>155</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>160</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>165</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>170</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>175</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>142</v>
+        <v>177</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>144</v>
+        <v>179</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>180</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>186</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>191</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>155</v>
+        <v>193</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>156</v>
+        <v>194</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>196</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>159</v>
+        <v>198</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>160</v>
+        <v>199</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>161</v>
+        <v>200</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>201</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>163</v>
+        <v>203</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>164</v>
+        <v>204</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>165</v>
+        <v>205</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>206</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>167</v>
+        <v>208</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>169</v>
+        <v>210</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>211</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>171</v>
+        <v>213</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>173</v>
+        <v>215</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>216</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>175</v>
+        <v>218</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>176</v>
+        <v>219</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>177</v>
+        <v>220</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>221</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>179</v>
+        <v>223</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>181</v>
+        <v>225</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>226</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>183</v>
+        <v>228</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>184</v>
+        <v>229</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>185</v>
+        <v>230</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>231</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>187</v>
+        <v>233</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>188</v>
+        <v>234</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>236</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>191</v>
+        <v>238</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>192</v>
+        <v>239</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>193</v>
+        <v>240</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>241</v>
+      </c>
+      <c r="I47" s="15" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>195</v>
+        <v>243</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>196</v>
+        <v>244</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>197</v>
+        <v>245</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+        <v>246</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>199</v>
+        <v>248</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>200</v>
+        <v>249</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+        <v>250</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="J49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>203</v>
+        <v>253</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>204</v>
+        <v>254</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>205</v>
+        <v>255</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+        <v>256</v>
+      </c>
+      <c r="I50" s="9" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>207</v>
+        <v>258</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>208</v>
+        <v>259</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>209</v>
+        <v>260</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+        <v>261</v>
+      </c>
+      <c r="I51" s="9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D52" s="2">
         <v>25</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>211</v>
+        <v>263</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>212</v>
+        <v>264</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="I52" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+        <v>265</v>
+      </c>
+      <c r="I52" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="J52" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D53" s="2">
         <v>26</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>214</v>
+        <v>267</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>215</v>
+        <v>268</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+        <v>269</v>
+      </c>
+      <c r="I53" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D54" s="2">
         <v>27</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>217</v>
+        <v>271</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>218</v>
+        <v>272</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>219</v>
+        <v>273</v>
+      </c>
+      <c r="I54" s="9" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>